<commit_message>
EPE - Experimental results are plotted for meeting.
</commit_message>
<xml_diff>
--- a/Project/3501/Furkan/Dataset/Dataset.xlsx
+++ b/Project/3501/Furkan/Dataset/Dataset.xlsx
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Teması">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -429,7 +429,7 @@
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,7 +472,7 @@
       <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -492,7 +492,7 @@
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -515,7 +515,7 @@
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -538,7 +538,7 @@
       <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C5" s="2" t="s">

</xml_diff>